<commit_message>
valve motion corrected nd new plots added
</commit_message>
<xml_diff>
--- a/relativePositionPistonValve.xlsx
+++ b/relativePositionPistonValve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Personal\CATA\02 FoU projekter\SPIRIT\stempel_kompressorer\pistonCompressorOperation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE91598-70DF-4A98-913F-95CAAC4948FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658B604D-1AEA-46AD-AD73-F557DE8E931A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -274,12 +274,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -294,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -302,13 +308,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +599,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +680,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -682,7 +689,7 @@
       <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>9.5399999999999999E-2</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -852,10 +859,6 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E13">
-        <f>L9+(L10-2*L11-L12)</f>
-        <v>9.9009999999999987E-2</v>
-      </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -867,10 +870,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E15" s="5">
-        <f>(L10-L12-2*L11)/2</f>
-        <v>1.999999999999999E-2</v>
-      </c>
+      <c r="E15" s="3"/>
       <c r="K15" t="s">
         <v>65</v>
       </c>
@@ -887,10 +887,7 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E17" s="5">
-        <f>D7+E15</f>
-        <v>7.9009999999999997E-2</v>
-      </c>
+      <c r="E17" s="3"/>
       <c r="K17" t="s">
         <v>69</v>
       </c>

</xml_diff>